<commit_message>
Booster, speedup and basic enemy scripts
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Status</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>Script Done. Need Model</t>
+  </si>
+  <si>
+    <t>Basic Script Ready</t>
   </si>
 </sst>
 </file>
@@ -2445,7 +2451,7 @@
   <dimension ref="B2:L39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2751,7 +2757,9 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="19" t="s">
+        <v>39</v>
+      </c>
       <c r="J21" s="5" t="b">
         <v>0</v>
       </c>
@@ -2801,7 +2809,9 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G23" s="19"/>
+      <c r="G23" s="19" t="s">
+        <v>39</v>
+      </c>
       <c r="J23" s="5" t="b">
         <v>0</v>
       </c>
@@ -2825,9 +2835,7 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G24" s="19" t="s">
-        <v>39</v>
-      </c>
+      <c r="G24" s="19"/>
       <c r="J24" s="5" t="b">
         <v>0</v>
       </c>
@@ -2877,7 +2885,9 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G26" s="19"/>
+      <c r="G26" s="19" t="s">
+        <v>40</v>
+      </c>
       <c r="J26" s="5" t="b">
         <v>0</v>
       </c>
@@ -2973,7 +2983,9 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G30" s="19"/>
+      <c r="G30" s="19" t="s">
+        <v>40</v>
+      </c>
       <c r="J30" s="5" t="b">
         <v>0</v>
       </c>
@@ -3021,9 +3033,7 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G32" s="19" t="s">
-        <v>39</v>
-      </c>
+      <c r="G32" s="19"/>
       <c r="J32" s="5" t="b">
         <v>0</v>
       </c>
@@ -3095,7 +3105,9 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G35" s="19"/>
+      <c r="G35" s="19" t="s">
+        <v>41</v>
+      </c>
       <c r="J35" s="5" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Enemy Model Complete and Sound
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -1,30 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jskinner2\Workspace\AGA206\Roll-A-Ball\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaxsk\Desktop\Projects\GitHub\Roll-A-Ball\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9697FCE-20C6-49FE-8101-7510DC73DBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="19080" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Status</t>
   </si>
@@ -144,9 +156,6 @@
   </si>
   <si>
     <t>y</t>
-  </si>
-  <si>
-    <t>Script Done. Need Model</t>
   </si>
   <si>
     <t>Basic Script Ready</t>
@@ -155,7 +164,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -316,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -329,7 +338,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -340,22 +348,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -370,22 +375,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -415,18 +411,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <strike/>
@@ -449,21 +434,12 @@
     </dxf>
     <dxf>
       <font>
-        <strike/>
+        <b/>
+        <i val="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -497,7 +473,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$26" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$26" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
@@ -513,7 +489,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$30" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$30" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,7 +553,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$22" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$22" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -603,6 +579,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1035"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -668,6 +647,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -732,6 +714,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -796,6 +781,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -860,6 +848,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1054"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -924,6 +915,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1055"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -988,6 +982,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1056"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1052,6 +1049,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1057"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1116,6 +1116,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1059"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1180,6 +1183,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1060"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1244,6 +1250,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1062"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1308,6 +1317,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1063"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1372,6 +1384,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1065"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1436,6 +1451,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1066"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1500,6 +1518,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1067"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1564,6 +1585,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1068"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1628,6 +1652,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1070"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1692,6 +1719,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1071"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1756,6 +1786,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1072"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1820,6 +1853,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1073"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1884,6 +1920,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1075"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1948,6 +1987,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1076"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2012,6 +2054,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1077"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2076,6 +2121,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1078"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000036040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2139,6 +2187,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1079"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2447,22 +2498,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.875" style="2" customWidth="1"/>
     <col min="2" max="2" width="6.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="23" customWidth="1"/>
+    <col min="3" max="3" width="29.625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="20" customWidth="1"/>
     <col min="5" max="5" width="7.625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="50.25" style="17" customWidth="1"/>
+    <col min="6" max="6" width="10.125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="50.25" style="14" customWidth="1"/>
     <col min="8" max="8" width="9.875" style="2" customWidth="1"/>
     <col min="9" max="9" width="10" style="2" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="5.125" style="2" hidden="1" customWidth="1"/>
@@ -2472,10 +2523,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="24" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2483,77 +2534,77 @@
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <f>COUNTIFS(J12:J15,TRUE)</f>
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="8">
         <f>K39</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="25" t="s">
+      <c r="E11" s="12"/>
+      <c r="F11" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="16" t="s">
         <v>3</v>
       </c>
       <c r="J11" s="3" t="s">
@@ -2561,127 +2612,122 @@
       </c>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>1</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="19">
         <v>0</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7" t="str">
+      <c r="E12" s="7"/>
+      <c r="F12" s="6" t="str">
         <f>IF(J12,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="G12" s="19"/>
+      <c r="G12" s="17"/>
       <c r="J12" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>2</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="19">
         <v>0</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="7" t="str">
+      <c r="E13" s="7"/>
+      <c r="F13" s="6" t="str">
         <f>IF(J13,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="G13" s="19"/>
+      <c r="G13" s="17"/>
       <c r="J13" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>3</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="19">
         <v>0</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="7" t="str">
+      <c r="E14" s="7"/>
+      <c r="F14" s="6" t="str">
         <f>IF(J14,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="G14" s="19"/>
+      <c r="G14" s="17"/>
       <c r="J14" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>4</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="19">
         <v>0</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="7" t="str">
+      <c r="E15" s="7"/>
+      <c r="F15" s="6" t="str">
         <f>IF(J15,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="G15" s="19"/>
+      <c r="G15" s="17"/>
       <c r="J15" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="10"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="26"/>
-      <c r="J16" s="6"/>
+      <c r="B16" s="9"/>
     </row>
     <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="20" t="s">
+      <c r="E17" s="11"/>
+      <c r="F17" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>5</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="19">
         <v>2</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="7" t="str">
+      <c r="E18" s="7"/>
+      <c r="F18" s="6" t="str">
         <f t="shared" ref="F18:F35" si="0">IF(J18,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="G18" s="19"/>
+      <c r="G18" s="17"/>
       <c r="J18" s="5" t="b">
         <v>1</v>
       </c>
@@ -2691,21 +2737,21 @@
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>6</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="19">
         <v>2</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="7" t="str">
+      <c r="E19" s="7"/>
+      <c r="F19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="17" t="s">
         <v>39</v>
       </c>
       <c r="J19" s="5" t="b">
@@ -2717,21 +2763,21 @@
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>7</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="19">
         <v>2</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="7" t="str">
+      <c r="E20" s="7"/>
+      <c r="F20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="17" t="s">
         <v>39</v>
       </c>
       <c r="J20" s="5" t="b">
@@ -2743,21 +2789,21 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>8</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="19">
         <v>2</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="7" t="str">
+      <c r="E21" s="7"/>
+      <c r="F21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="17" t="s">
         <v>39</v>
       </c>
       <c r="J21" s="5" t="b">
@@ -2769,47 +2815,45 @@
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>9</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="19">
         <v>1</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="7" t="str">
+      <c r="E22" s="7"/>
+      <c r="F22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="G22" s="17"/>
+      <c r="J22" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="6">
+        <v>10</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="19">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G22" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="J22" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="7">
-        <v>10</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="21">
-        <v>1</v>
-      </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="17" t="s">
         <v>39</v>
       </c>
       <c r="J23" s="5" t="b">
@@ -2821,21 +2865,21 @@
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <v>11</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="19">
         <v>1</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="7" t="str">
+      <c r="E24" s="7"/>
+      <c r="F24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G24" s="19"/>
+      <c r="G24" s="17"/>
       <c r="J24" s="5" t="b">
         <v>0</v>
       </c>
@@ -2845,21 +2889,21 @@
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <v>12</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="19">
         <v>1</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="7" t="str">
+      <c r="E25" s="7"/>
+      <c r="F25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="17" t="s">
         <v>39</v>
       </c>
       <c r="J25" s="5" t="b">
@@ -2871,47 +2915,47 @@
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <v>13</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="19">
         <v>1</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="7" t="str">
+      <c r="E26" s="7"/>
+      <c r="F26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="G26" s="17"/>
+      <c r="J26" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="6">
+        <v>14</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="19">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G26" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="J26" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="7">
-        <v>14</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="21">
-        <v>1</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="J27" s="5" t="b">
         <v>0</v>
       </c>
@@ -2921,21 +2965,21 @@
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="7">
+      <c r="B28" s="6">
         <v>15</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="21">
+      <c r="D28" s="19">
         <v>1</v>
       </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="7" t="str">
+      <c r="E28" s="7"/>
+      <c r="F28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G28" s="19"/>
+      <c r="G28" s="17"/>
       <c r="J28" s="5" t="b">
         <v>0</v>
       </c>
@@ -2945,21 +2989,21 @@
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="7">
+      <c r="B29" s="6">
         <v>16</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="21">
+      <c r="D29" s="19">
         <v>1</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="7" t="str">
+      <c r="E29" s="7"/>
+      <c r="F29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G29" s="19"/>
+      <c r="G29" s="17"/>
       <c r="J29" s="5" t="b">
         <v>0</v>
       </c>
@@ -2969,47 +3013,45 @@
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="7">
+      <c r="B30" s="6">
         <v>17</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="21">
+      <c r="D30" s="19">
         <v>1</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="7" t="str">
+      <c r="E30" s="7"/>
+      <c r="F30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="G30" s="17"/>
+      <c r="J30" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B31" s="6">
+        <v>18</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="19">
+        <v>1</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G30" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="J30" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K30" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="7">
-        <v>18</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="21">
-        <v>1</v>
-      </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G31" s="19"/>
+      <c r="G31" s="17"/>
       <c r="J31" s="5" t="b">
         <v>0</v>
       </c>
@@ -3019,21 +3061,21 @@
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="7">
+      <c r="B32" s="6">
         <v>19</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="19">
         <v>1</v>
       </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="7" t="str">
+      <c r="E32" s="7"/>
+      <c r="F32" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G32" s="19"/>
+      <c r="G32" s="17"/>
       <c r="J32" s="5" t="b">
         <v>0</v>
       </c>
@@ -3043,21 +3085,21 @@
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B33" s="7">
+      <c r="B33" s="6">
         <v>20</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="21">
+      <c r="D33" s="19">
         <v>1</v>
       </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="7" t="str">
+      <c r="E33" s="7"/>
+      <c r="F33" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G33" s="19"/>
+      <c r="G33" s="17"/>
       <c r="J33" s="5" t="b">
         <v>0</v>
       </c>
@@ -3067,21 +3109,21 @@
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B34" s="7">
+      <c r="B34" s="6">
         <v>21</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="21">
+      <c r="D34" s="19">
         <v>2</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="7" t="str">
+      <c r="E34" s="7"/>
+      <c r="F34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="G34" s="19"/>
+      <c r="G34" s="17"/>
       <c r="J34" s="5" t="b">
         <v>1</v>
       </c>
@@ -3091,22 +3133,22 @@
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B35" s="7">
+      <c r="B35" s="6">
         <v>22</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="21">
+      <c r="D35" s="19">
         <v>1</v>
       </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="7" t="str">
+      <c r="E35" s="7"/>
+      <c r="F35" s="6" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G35" s="19" t="s">
-        <v>41</v>
+      <c r="G35" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="J35" s="5" t="b">
         <v>0</v>
@@ -3117,21 +3159,21 @@
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B36" s="7">
+      <c r="B36" s="6">
         <v>23</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="19">
         <v>2</v>
       </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="7" t="str">
+      <c r="E36" s="7"/>
+      <c r="F36" s="6" t="str">
         <f t="shared" ref="F36:F38" si="2">IF(J36,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="G36" s="19"/>
+      <c r="G36" s="17"/>
       <c r="J36" s="5" t="b">
         <v>0</v>
       </c>
@@ -3141,21 +3183,21 @@
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B37" s="7">
+      <c r="B37" s="6">
         <v>24</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="21">
+      <c r="D37" s="19">
         <v>1</v>
       </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="7" t="str">
+      <c r="E37" s="7"/>
+      <c r="F37" s="6" t="str">
         <f t="shared" si="2"/>
         <v>To Be Done</v>
       </c>
-      <c r="G37" s="19"/>
+      <c r="G37" s="17"/>
       <c r="J37" s="5" t="b">
         <v>0</v>
       </c>
@@ -3165,21 +3207,21 @@
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B38" s="7">
+      <c r="B38" s="6">
         <v>25</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D38" s="21">
+      <c r="D38" s="19">
         <v>1</v>
       </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="7" t="str">
+      <c r="E38" s="7"/>
+      <c r="F38" s="6" t="str">
         <f t="shared" si="2"/>
         <v>To Be Done</v>
       </c>
-      <c r="G38" s="19"/>
+      <c r="G38" s="17"/>
       <c r="J38" s="5" t="b">
         <v>0</v>
       </c>
@@ -3191,7 +3233,7 @@
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -3199,33 +3241,23 @@
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="D4:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="F22:F23 F26:F29 F12:F16 F34:F38">
-    <cfRule type="expression" dxfId="4" priority="10">
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThanOrEqual">
+      <formula>14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:F16">
+    <cfRule type="expression" dxfId="1" priority="10">
       <formula>$F12="Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18:F21">
-    <cfRule type="expression" dxfId="3" priority="8">
+  <conditionalFormatting sqref="F18:F38">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>$F18="Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F24:F25">
-    <cfRule type="expression" dxfId="2" priority="7">
-      <formula>$F24="Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F30:F33">
-    <cfRule type="expression" dxfId="1" priority="6">
-      <formula>$F30="Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
-      <formula>14</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Clean Up for Assessment
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaxsk\Desktop\Projects\GitHub\Roll-A-Ball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96ED6128-749A-47F9-96DB-7A32F0ACEC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2FB8B1-3A28-49EB-8B4E-0CBB0B7A502F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1455" yWindow="1260" windowWidth="14400" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>Status</t>
   </si>
@@ -150,12 +150,6 @@
   </si>
   <si>
     <t>https://github.com/Valgius/Roll-A-Ball</t>
-  </si>
-  <si>
-    <t>Starting Cutscene</t>
-  </si>
-  <si>
-    <t>Image Stills with Skip Button</t>
   </si>
   <si>
     <t>Stairs. Destructable Barrels and Doors.</t>
@@ -437,6 +431,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -452,20 +460,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2563,7 +2557,7 @@
   <dimension ref="B2:L39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2598,12 +2592,12 @@
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="31"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
     </row>
@@ -2611,12 +2605,12 @@
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="31"/>
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
     </row>
@@ -2837,7 +2831,7 @@
         <v>Done</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J20" s="5" t="b">
         <v>1</v>
@@ -2959,7 +2953,7 @@
         <v>Done</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J25" s="5" t="b">
         <v>1</v>
@@ -3129,7 +3123,7 @@
         <v>Done</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J32" s="5" t="b">
         <v>1</v>
@@ -3178,9 +3172,7 @@
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="G34" s="30" t="s">
-        <v>39</v>
-      </c>
+      <c r="G34" s="26"/>
       <c r="J34" s="5" t="b">
         <v>1</v>
       </c>
@@ -3194,17 +3186,17 @@
         <v>22</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D35" s="19">
         <v>1</v>
       </c>
       <c r="E35" s="7"/>
-      <c r="F35" s="29" t="str">
+      <c r="F35" s="25" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G35" s="32"/>
+      <c r="G35" s="28"/>
       <c r="J35" s="5" t="b">
         <v>0</v>
       </c>
@@ -3224,11 +3216,11 @@
         <v>1</v>
       </c>
       <c r="E36" s="7"/>
-      <c r="F36" s="29" t="str">
+      <c r="F36" s="25" t="str">
         <f t="shared" ref="F36:F38" si="2">IF(J36,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="G36" s="32"/>
+      <c r="G36" s="28"/>
       <c r="J36" s="5" t="b">
         <v>0</v>
       </c>
@@ -3252,7 +3244,7 @@
         <f t="shared" si="2"/>
         <v>To Be Done</v>
       </c>
-      <c r="G37" s="31"/>
+      <c r="G37" s="27"/>
       <c r="J37" s="5" t="b">
         <v>0</v>
       </c>

</xml_diff>